<commit_message>
1. Add a "Screen Definition" page. 2.Allow dragging and dropping of multi-selected cells, starting from the dateBox.
</commit_message>
<xml_diff>
--- a/apps/demo/djn/var/sys/views/demo/UploadAndDownloadDemo-v0.xlsx
+++ b/apps/demo/djn/var/sys/views/demo/UploadAndDownloadDemo-v0.xlsx
@@ -348,9 +348,6 @@
     <t>File</t>
   </si>
   <si>
-    <t>multiple:yes</t>
-  </si>
-  <si>
     <t>importBtt1</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>One tailor made javascript for each layout</t>
+  </si>
+  <si>
+    <t>multiple:true</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1643,7 +1643,7 @@
         <v>101</v>
       </c>
       <c r="J35" s="12" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
@@ -1657,7 +1657,7 @@
         <v>76</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>75</v>
@@ -1666,16 +1666,16 @@
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J36" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="J36" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
       <c r="N36" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
@@ -1685,7 +1685,7 @@
         <v>78</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>100</v>
@@ -1697,7 +1697,7 @@
         <v>101</v>
       </c>
       <c r="J37" s="12" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
@@ -1711,7 +1711,7 @@
         <v>80</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>79</v>
@@ -1720,16 +1720,16 @@
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
       <c r="I38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J38" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
@@ -1739,25 +1739,25 @@
         <v>81</v>
       </c>
       <c r="D39" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="12"/>
       <c r="H39" s="12"/>
       <c r="I39" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J39" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
@@ -1765,25 +1765,25 @@
     <row r="40" spans="1:16">
       <c r="C40" s="12"/>
       <c r="D40" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J40" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
       <c r="N40" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
@@ -1808,13 +1808,13 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>57</v>
@@ -1840,22 +1840,22 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>35</v>
@@ -1879,15 +1879,15 @@
     </row>
     <row r="56" spans="1:11">
       <c r="B56" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="19" t="s">
@@ -1897,22 +1897,22 @@
         <v>94</v>
       </c>
       <c r="E57" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F57" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="G57" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="G57" s="19" t="s">
+      <c r="H57" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>131</v>
       </c>
       <c r="I57" s="19" t="s">
         <v>35</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -1924,7 +1924,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
       <c r="K58" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -1980,7 +1980,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>